<commit_message>
corretti casi d'uso id 18,19,20,21,22,23
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS/P4PVACCINAZIONI/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS/P4PVACCINAZIONI/1.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\massimo.musante\git\ServiziFSE2\ServiziFSE2\pull-request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B349E46-2DB8-4E92-8CD7-9F9C443B36C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BED7FFB-BF1C-4FF0-89EA-67AC84E1A67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -958,58 +958,58 @@
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.91718fd0a94b37eccfd78bfddb36b3a1f843de4d3abf1563c59a05c0da5ae816.f92f6cabbb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>80bd12e7d578c899</t>
-  </si>
-  <si>
-    <t>2023-05-17T12:58:46Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.414adb0dd796b1816d7ee39d9f95e84ab5378ccdc996c0399717dd50dda4d44e.d5498c8b07^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-17T14:45:02Z</t>
-  </si>
-  <si>
-    <t>2f6b105a68763537</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.cd35ca59f0dd85533f06acbfee1a69a983aee265709aea36763488a83aeaef39.4fcbd71c8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-17T15:18:29Z</t>
-  </si>
-  <si>
-    <t>fe143fec4393f19e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.f80e6ffde4f9ac339fa3f481df7c4ae5064077543cf6b6a08620f45e40ecd3b3.94a0ccabc9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-17T15:23:37Z</t>
-  </si>
-  <si>
-    <t>485540a600405aaf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a9eda353cf983ce373410f0a65c7e7fb82ecf94637b23a2b62c396be8e11181b.cfdcc1a7a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-17T15:58:37Z</t>
-  </si>
-  <si>
-    <t>5ad51d55ba1d0f2d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.403d4d62c06f6b133ae8ae3824e2720633ae00fafbff1ec6041f226584754566.a93bc812f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-17T16:04:00Z</t>
-  </si>
-  <si>
-    <t>3027d68ee5386d38</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.3a4dade1a26fcba6e1f5bd6199312571d5c64de730a7409e8dc705bccf1de9e6.648ff8ead5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-05-19T17:47:05Z</t>
+  </si>
+  <si>
+    <t>b8fad2c8c65f8ac2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.d563f27a72d11274d252dbcb1caa8321e1283a6d3af52fd15cfe5bbc295daa86.08e3319519^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-19T17:50:56Z</t>
+  </si>
+  <si>
+    <t>a2403033625acfd3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.8389b074dd92b46208ccdb823614aba1b65728984bca406a8a1cf4a007b0329f.c8e08496bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-19T17:54:22Z</t>
+  </si>
+  <si>
+    <t>534082409f2e6607</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.2f4aa7b96c9bec33639ce08e14332dff0100b7443ce34d8fac01f6d50893474a.24ad7fd78f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-19T17:57:36Z</t>
+  </si>
+  <si>
+    <t>8636215e9f7ed6c1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.16dd6296c7a73cdc68da5243b659f9026ea5b9ef55ae05ab0638eeb564cc6364.40ed7f9b98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-19T17:59:39Z</t>
+  </si>
+  <si>
+    <t>d43e31b4b9ebb32c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.409f4a915636fc8edc8c9b02a722286f9eca43a11d7da9e2e720a9acfe849f50.dcb0081780^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-19T18:02:47Z</t>
+  </si>
+  <si>
+    <t>99fbff95df71cbb2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.32c2b60f1c38d01282ad4d4efd5833bb7de8f6be68679c9b6e5a96416cddc8b9.855656404b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1437,6 +1437,9 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1458,9 +1461,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3961,12 +3961,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="39"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3984,14 +3984,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="39"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4009,12 +4009,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="46" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4033,12 +4033,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="39"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4056,8 +4056,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4196,7 +4196,7 @@
       <c r="G10" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="35" t="s">
         <v>202</v>
       </c>
       <c r="I10" s="32" t="s">
@@ -4279,13 +4279,13 @@
         <v>54</v>
       </c>
       <c r="F12" s="23">
-        <v>45063</v>
+        <v>45065</v>
       </c>
       <c r="G12" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>208</v>
-      </c>
-      <c r="H12" s="32" t="s">
-        <v>207</v>
       </c>
       <c r="I12" s="32" t="s">
         <v>209</v>
@@ -4323,7 +4323,7 @@
         <v>56</v>
       </c>
       <c r="F13" s="23">
-        <v>45063</v>
+        <v>45065</v>
       </c>
       <c r="G13" s="32" t="s">
         <v>210</v>
@@ -4367,7 +4367,7 @@
         <v>58</v>
       </c>
       <c r="F14" s="23">
-        <v>45063</v>
+        <v>45065</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>213</v>
@@ -4411,7 +4411,7 @@
         <v>60</v>
       </c>
       <c r="F15" s="23">
-        <v>45063</v>
+        <v>45065</v>
       </c>
       <c r="G15" s="32" t="s">
         <v>216</v>
@@ -4455,7 +4455,7 @@
         <v>62</v>
       </c>
       <c r="F16" s="23">
-        <v>45063</v>
+        <v>45065</v>
       </c>
       <c r="G16" s="32" t="s">
         <v>219</v>
@@ -4499,7 +4499,7 @@
         <v>64</v>
       </c>
       <c r="F17" s="23">
-        <v>45063</v>
+        <v>45065</v>
       </c>
       <c r="G17" s="32" t="s">
         <v>222</v>

</xml_diff>

<commit_message>
Chiarimento su ID 49, 50
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS/P4PVACCINAZIONI/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS/P4PVACCINAZIONI/1.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\massimo.musante\git\ServiziFSE2\ServiziFSE2\pull-request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BED7FFB-BF1C-4FF0-89EA-67AC84E1A67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871A2672-704F-4125-B12E-2F52A37EAA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -787,9 +787,6 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>Viene segnalato un errore di timeout della validazione e si richiede all'utente di riprovare in un successivo momento</t>
-  </si>
-  <si>
     <t>Viene mostrato l'errore di ritorno dal gateway di validazione</t>
   </si>
   <si>
@@ -1010,6 +1007,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.32c2b60f1c38d01282ad4d4efd5833bb7de8f6be68679c9b6e5a96416cddc8b9.855656404b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di timeout della validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nel programma una modalità "cruscotto" che permette di reinviare le eventuali validazioni fallite</t>
   </si>
 </sst>
 </file>
@@ -3919,10 +3919,10 @@
   <dimension ref="A1:T669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="L22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="B3" s="42"/>
       <c r="C3" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D3" s="39"/>
       <c r="F3" s="12"/>
@@ -4036,7 +4036,7 @@
       <c r="A5" s="45"/>
       <c r="B5" s="46"/>
       <c r="C5" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="39"/>
       <c r="F5" s="12"/>
@@ -4194,13 +4194,13 @@
         <v>45063</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H10" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="I10" s="32" t="s">
         <v>202</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>203</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>73</v>
@@ -4238,13 +4238,13 @@
         <v>45063</v>
       </c>
       <c r="G11" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="I11" s="32" t="s">
         <v>205</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>206</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>73</v>
@@ -4282,13 +4282,13 @@
         <v>45065</v>
       </c>
       <c r="G12" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="I12" s="32" t="s">
         <v>208</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>209</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>73</v>
@@ -4326,13 +4326,13 @@
         <v>45065</v>
       </c>
       <c r="G13" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="I13" s="32" t="s">
         <v>211</v>
-      </c>
-      <c r="I13" s="32" t="s">
-        <v>212</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>73</v>
@@ -4370,13 +4370,13 @@
         <v>45065</v>
       </c>
       <c r="G14" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="H14" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="I14" s="32" t="s">
         <v>214</v>
-      </c>
-      <c r="I14" s="32" t="s">
-        <v>215</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>73</v>
@@ -4414,13 +4414,13 @@
         <v>45065</v>
       </c>
       <c r="G15" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="H15" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="H15" s="32" t="s">
+      <c r="I15" s="32" t="s">
         <v>217</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>218</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>73</v>
@@ -4458,13 +4458,13 @@
         <v>45065</v>
       </c>
       <c r="G16" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="H16" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="I16" s="32" t="s">
         <v>220</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>221</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>73</v>
@@ -4502,13 +4502,13 @@
         <v>45065</v>
       </c>
       <c r="G17" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="H17" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="I17" s="32" t="s">
         <v>223</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>224</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>73</v>
@@ -4546,10 +4546,10 @@
         <v>45041</v>
       </c>
       <c r="G18" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>198</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>199</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>149</v>
@@ -4565,13 +4565,13 @@
         <v>73</v>
       </c>
       <c r="N18" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O18" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -4600,10 +4600,10 @@
         <v>45041</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I19" s="24" t="s">
         <v>149</v>
@@ -4619,13 +4619,13 @@
         <v>73</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -4654,10 +4654,10 @@
         <v>45041</v>
       </c>
       <c r="G20" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="H20" s="24" t="s">
         <v>196</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>197</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>149</v>
@@ -4673,13 +4673,13 @@
         <v>73</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4708,10 +4708,10 @@
         <v>45041</v>
       </c>
       <c r="G21" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" s="32" t="s">
         <v>194</v>
-      </c>
-      <c r="H21" s="32" t="s">
-        <v>195</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>149</v>
@@ -4727,13 +4727,13 @@
         <v>73</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -4742,7 +4742,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="75.75" thickBot="1">
+    <row r="22" spans="1:20" ht="135.75" thickBot="1">
       <c r="A22" s="20">
         <v>49</v>
       </c>
@@ -4769,7 +4769,7 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="33" t="s">
-        <v>150</v>
+        <v>224</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26" t="s">
@@ -4780,7 +4780,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="75.75" thickBot="1">
+    <row r="23" spans="1:20" ht="135.75" thickBot="1">
       <c r="A23" s="20">
         <v>50</v>
       </c>
@@ -4807,7 +4807,7 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="33" t="s">
-        <v>150</v>
+        <v>224</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="26" t="s">
@@ -4838,13 +4838,13 @@
         <v>45041</v>
       </c>
       <c r="G24" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="H24" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="I24" s="24" t="s">
         <v>157</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>158</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>73</v>
@@ -4857,13 +4857,13 @@
         <v>73</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O24" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="26"/>
@@ -4892,13 +4892,13 @@
         <v>45041</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>73</v>
@@ -4911,13 +4911,13 @@
         <v>73</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O25" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="26"/>
@@ -4988,7 +4988,7 @@
         <v>141</v>
       </c>
       <c r="K27" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
@@ -5174,13 +5174,13 @@
         <v>45041</v>
       </c>
       <c r="G32" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H32" s="24" t="s">
+      <c r="I32" s="24" t="s">
         <v>163</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>164</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>73</v>
@@ -5193,13 +5193,13 @@
         <v>73</v>
       </c>
       <c r="N32" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O32" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P32" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="26"/>
@@ -5228,13 +5228,13 @@
         <v>45041</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H33" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="I33" s="24" t="s">
         <v>165</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>166</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>73</v>
@@ -5247,13 +5247,13 @@
         <v>73</v>
       </c>
       <c r="N33" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O33" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P33" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="26"/>
@@ -5282,13 +5282,13 @@
         <v>45041</v>
       </c>
       <c r="G34" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H34" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="H34" s="24" t="s">
+      <c r="I34" s="24" t="s">
         <v>169</v>
-      </c>
-      <c r="I34" s="24" t="s">
-        <v>170</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>73</v>
@@ -5301,13 +5301,13 @@
         <v>73</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O34" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P34" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5378,7 +5378,7 @@
         <v>141</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -5412,13 +5412,13 @@
         <v>45041</v>
       </c>
       <c r="G37" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="I37" s="24" t="s">
         <v>173</v>
-      </c>
-      <c r="I37" s="24" t="s">
-        <v>174</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>73</v>
@@ -5431,13 +5431,13 @@
         <v>73</v>
       </c>
       <c r="N37" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O37" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -5466,13 +5466,13 @@
         <v>45041</v>
       </c>
       <c r="G38" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="I38" s="24" t="s">
         <v>176</v>
-      </c>
-      <c r="I38" s="24" t="s">
-        <v>177</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>73</v>
@@ -5485,13 +5485,13 @@
         <v>73</v>
       </c>
       <c r="N38" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O38" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P38" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="26"/>
@@ -5561,7 +5561,7 @@
         <v>141</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L40" s="25"/>
       <c r="M40" s="25"/>
@@ -5570,7 +5570,7 @@
         <v>73</v>
       </c>
       <c r="P40" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="26"/>
@@ -5713,13 +5713,13 @@
         <v>45041</v>
       </c>
       <c r="G44" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="H44" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="H44" s="34" t="s">
+      <c r="I44" s="24" t="s">
         <v>179</v>
-      </c>
-      <c r="I44" s="24" t="s">
-        <v>180</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>73</v>
@@ -5732,13 +5732,13 @@
         <v>73</v>
       </c>
       <c r="N44" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O44" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P44" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="26"/>
@@ -5805,13 +5805,13 @@
         <v>45041</v>
       </c>
       <c r="G46" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="H46" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="H46" s="32" t="s">
+      <c r="I46" s="32" t="s">
         <v>182</v>
-      </c>
-      <c r="I46" s="32" t="s">
-        <v>183</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>73</v>
@@ -5824,13 +5824,13 @@
         <v>73</v>
       </c>
       <c r="N46" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P46" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
@@ -5859,13 +5859,13 @@
         <v>45041</v>
       </c>
       <c r="G47" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="H47" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="I47" s="24" t="s">
         <v>185</v>
-      </c>
-      <c r="I47" s="24" t="s">
-        <v>186</v>
       </c>
       <c r="J47" s="33" t="s">
         <v>73</v>
@@ -5878,13 +5878,13 @@
         <v>73</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -5913,13 +5913,13 @@
         <v>45041</v>
       </c>
       <c r="G48" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="H48" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="H48" s="24" t="s">
+      <c r="I48" s="24" t="s">
         <v>188</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>189</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>73</v>
@@ -5932,13 +5932,13 @@
         <v>73</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P48" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="26"/>
@@ -6005,13 +6005,13 @@
         <v>45041</v>
       </c>
       <c r="G50" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="H50" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="H50" s="24" t="s">
+      <c r="I50" s="32" t="s">
         <v>191</v>
-      </c>
-      <c r="I50" s="32" t="s">
-        <v>192</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>73</v>
@@ -6024,13 +6024,13 @@
         <v>73</v>
       </c>
       <c r="N50" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O50" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P50" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="26"/>
@@ -6063,7 +6063,7 @@
         <v>141</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L51" s="25"/>
       <c r="M51" s="25"/>

</xml_diff>